<commit_message>
Add requirements.txt, fix responsive layout
</commit_message>
<xml_diff>
--- a/server/data/anime_characters.xlsx
+++ b/server/data/anime_characters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHMT\2024-2025\HK1\Niên luận ngành\Akinator_Vue\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B035C45-F400-46E8-B6D2-51CB470BAB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C4EEA1-C0CD-4F00-9638-2F080B39C834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DCA09FA5-3F54-4DF3-A744-A79B62034746}"/>
+    <workbookView xWindow="60" yWindow="576" windowWidth="21744" windowHeight="10728" xr2:uid="{DCA09FA5-3F54-4DF3-A744-A79B62034746}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -997,10 +997,10 @@
   <dimension ref="A1:BW105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BP30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>